<commit_message>
Hecho entregable y terminada memoria
</commit_message>
<xml_diff>
--- a/P4/Docs/E3.xlsx
+++ b/P4/Docs/E3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\tugfa123\Practicas\Practicas_ARQO\P4\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2139DF67-1B80-451F-97E3-9D54C7AF9DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8186C85-35D3-41A6-BF72-0AAD4082BCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="6210" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{6E0C4A6B-219A-4CC3-9C09-32EDF042FF6A}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15345" xr2:uid="{6E0C4A6B-219A-4CC3-9C09-32EDF042FF6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -213,11 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC673AEA-F19D-4108-8B14-BC88E6B32454}">
   <dimension ref="D7:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,13 +566,13 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="J7" t="s">
         <v>7</v>
       </c>
@@ -663,13 +663,13 @@
       </c>
     </row>
     <row r="16" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
@@ -788,17 +788,17 @@
   </cols>
   <sheetData>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C715C7-3437-4B89-AA39-94D8E3733D80}">
   <dimension ref="D5:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +939,7 @@
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1">
@@ -959,7 +959,7 @@
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1">
@@ -979,7 +979,7 @@
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1">
@@ -1004,7 +1004,7 @@
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="1">
@@ -1029,7 +1029,7 @@
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="1">

</xml_diff>